<commit_message>
new invalid CSV lines
</commit_message>
<xml_diff>
--- a/src/test/resources/invalidCSV/input/instructions.xlsx
+++ b/src/test/resources/invalidCSV/input/instructions.xlsx
@@ -1,19 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/invalidCSV/input/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38640" windowHeight="21840" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AZ$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BB$4</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="119">
   <si>
     <t>DATASET</t>
   </si>
@@ -358,6 +366,27 @@
   </si>
   <si>
     <t>SF_PLAY_MODE</t>
+  </si>
+  <si>
+    <t>DCT_DATE</t>
+  </si>
+  <si>
+    <t>DCT_DATE_QUALIFIER</t>
+  </si>
+  <si>
+    <t>Text with Qualifier</t>
+  </si>
+  <si>
+    <t>ISSUED</t>
+  </si>
+  <si>
+    <t>30-07-1992</t>
+  </si>
+  <si>
+    <t>vAlId</t>
+  </si>
+  <si>
+    <t>modiFied</t>
   </si>
 </sst>
 </file>
@@ -367,7 +396,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -412,6 +441,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -553,14 +589,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -588,13 +627,21 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
+  <cellStyles count="8">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -861,7 +908,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -869,72 +916,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA4"/>
+  <dimension ref="A1:BC4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV1" sqref="AV1"/>
+      <selection pane="bottomRight" activeCell="AL4" sqref="AL4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="50.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="26" max="27" width="14" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="65.625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.875" customWidth="1"/>
-    <col min="49" max="49" width="47.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="29.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="40.375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="23" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.1640625" customWidth="1"/>
+    <col min="38" max="38" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="17.83203125" customWidth="1"/>
+    <col min="51" max="51" width="47.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="29.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="23" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1043,59 +1092,65 @@
       <c r="AJ1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AK1" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="AM1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AV1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AY1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="BA1" s="20" t="s">
+      <c r="BC1" s="20" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:53" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>43</v>
       </c>
@@ -1184,47 +1239,53 @@
         <v>88</v>
       </c>
       <c r="AJ2" s="10"/>
-      <c r="AK2" s="7" t="s">
+      <c r="AK2" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="AL2" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="AM2" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="AL2" s="7" t="s">
+      <c r="AN2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AO2" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AN2" s="7" t="s">
+      <c r="AP2" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="AO2" s="11" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="AP2" s="8">
+      <c r="AR2" s="8">
         <v>33815</v>
-      </c>
-      <c r="AQ2" s="11"/>
-      <c r="AR2" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="AS2" s="11"/>
       <c r="AT2" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="AU2" s="7" t="s">
+      <c r="AW2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="11" t="s">
+      <c r="AX2" s="7"/>
+      <c r="AY2" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="AX2" s="11"/>
-      <c r="AY2" s="7"/>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="21" t="s">
+      <c r="AZ2" s="11"/>
+      <c r="BA2" s="7"/>
+      <c r="BB2" s="7"/>
+      <c r="BC2" s="21" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>43</v>
       </c>
@@ -1299,39 +1360,43 @@
         <v>89</v>
       </c>
       <c r="AJ3" s="13"/>
-      <c r="AK3" s="13"/>
-      <c r="AL3" s="13" t="s">
+      <c r="AK3" s="25"/>
+      <c r="AL3" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM3" s="13"/>
+      <c r="AN3" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="AM3" s="13" t="s">
+      <c r="AO3" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="AN3" s="13"/>
-      <c r="AO3" s="15" t="s">
+      <c r="AP3" s="13"/>
+      <c r="AQ3" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="AP3" s="15" t="s">
+      <c r="AR3" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="AQ3" s="15" t="s">
+      <c r="AS3" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="AR3" s="16"/>
-      <c r="AS3" s="16"/>
       <c r="AT3" s="16"/>
-      <c r="AU3" s="13"/>
-      <c r="AV3" s="13"/>
-      <c r="AW3" s="15"/>
-      <c r="AX3" s="15" t="s">
+      <c r="AU3" s="16"/>
+      <c r="AV3" s="16"/>
+      <c r="AW3" s="13"/>
+      <c r="AX3" s="13"/>
+      <c r="AY3" s="15"/>
+      <c r="AZ3" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="AY3" s="13"/>
-      <c r="AZ3" s="13"/>
-      <c r="BA3" s="22" t="s">
+      <c r="BA3" s="13"/>
+      <c r="BB3" s="13"/>
+      <c r="BC3" s="22" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:53" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>43</v>
       </c>
@@ -1378,25 +1443,31 @@
       <c r="AJ4" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="AK4" s="13"/>
-      <c r="AL4" s="13" t="s">
+      <c r="AK4" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL4" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="AM4" s="13"/>
-      <c r="AN4" s="13"/>
-      <c r="AO4" s="15"/>
-      <c r="AP4" s="15"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13"/>
       <c r="AQ4" s="15"/>
       <c r="AR4" s="15"/>
       <c r="AS4" s="15"/>
       <c r="AT4" s="15"/>
-      <c r="AU4" s="13"/>
-      <c r="AV4" s="13"/>
-      <c r="AW4" s="15"/>
-      <c r="AX4" s="15"/>
-      <c r="AY4" s="13"/>
-      <c r="AZ4" s="13"/>
-      <c r="BA4" s="17"/>
+      <c r="AU4" s="15"/>
+      <c r="AV4" s="15"/>
+      <c r="AW4" s="13"/>
+      <c r="AX4" s="13"/>
+      <c r="AY4" s="15"/>
+      <c r="AZ4" s="15"/>
+      <c r="BA4" s="13"/>
+      <c r="BB4" s="13"/>
+      <c r="BC4" s="17"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
EASY-1479: dcterms:spatial should also accept the ISO3166 country codes (#153)
</commit_message>
<xml_diff>
--- a/src/test/resources/invalidCSV/input/instructions.xlsx
+++ b/src/test/resources/invalidCSV/input/instructions.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RichardvanHeest/git/service/easy/easy-split-multi-deposit/src/test/resources/invalidCSV/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vesaakerman/git/service/easy/easy-split-multi-deposit/src/test/resources/invalidCSV/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4034159-4C68-924F-BB09-4D7C8CBF021D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C0D300-9E59-464E-B823-67F4D461B37B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26260" windowHeight="16260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BC$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$BD$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="123">
   <si>
     <t>DATASET</t>
   </si>
@@ -273,9 +273,6 @@
     <t>here</t>
   </si>
   <si>
-    <t>there</t>
-  </si>
-  <si>
     <t>RD</t>
   </si>
   <si>
@@ -388,6 +385,21 @@
   </si>
   <si>
     <t>http://x</t>
+  </si>
+  <si>
+    <t>DCT_SPATIAL_SCHEME</t>
+  </si>
+  <si>
+    <t>dcterms:ISO3177</t>
+  </si>
+  <si>
+    <t>dcterms:ISO3166</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>XYZ</t>
   </si>
 </sst>
 </file>
@@ -397,7 +409,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -469,6 +481,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -640,7 +658,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -679,6 +697,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -975,13 +994,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BE4"/>
+  <dimension ref="A1:BF4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ5" sqref="AJ5"/>
+      <selection pane="bottomRight" activeCell="Z10" sqref="Z10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,42 +1028,43 @@
     <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="14" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="18.1640625" customWidth="1"/>
-    <col min="38" max="38" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="65.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="36.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="17.83203125" customWidth="1"/>
-    <col min="53" max="53" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="31.83203125" customWidth="1"/>
+    <col min="24" max="24" width="22.33203125" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.1640625" customWidth="1"/>
+    <col min="39" max="39" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="15.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="36.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.83203125" customWidth="1"/>
+    <col min="54" max="54" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1114,110 +1134,113 @@
       <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="X1" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AH1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="21" t="s">
+      <c r="AL1" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="AM1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="AL1" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AR1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AS1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AT1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="AV1" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AW1" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="AV1" s="29" t="s">
+      <c r="AX1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="BB1" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="AW1" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="AX1" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="AY1" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AZ1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="BA1" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="BB1" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="BC1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="BD1" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="BD1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="BE1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="BE1" s="31" t="s">
-        <v>116</v>
+      <c r="BF1" s="31" t="s">
+        <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:57" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>43</v>
       </c>
@@ -1252,13 +1275,13 @@
         <v>74</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="O2" s="7" t="s">
         <v>77</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="Q2" s="10"/>
       <c r="R2" s="7" t="s">
@@ -1277,82 +1300,83 @@
       <c r="W2" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="Y2" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="Z2" s="7">
+      <c r="Z2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA2" s="7">
         <v>83575.399999999994</v>
       </c>
-      <c r="AA2" s="7">
+      <c r="AB2" s="7">
         <v>455271.2</v>
       </c>
-      <c r="AB2" s="7"/>
       <c r="AC2" s="7"/>
       <c r="AD2" s="7"/>
       <c r="AE2" s="7"/>
-      <c r="AF2" s="10" t="s">
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="AI2" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="22" t="s">
+      <c r="AJ2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="AM2" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="AL2" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AN2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AP2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ2" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="AN2" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AO2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP2" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="AQ2" s="10" t="s">
+      <c r="AR2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="AR2" s="8">
+      <c r="AS2" s="8">
         <v>33815</v>
       </c>
-      <c r="AS2" s="10"/>
-      <c r="AT2" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="AU2" s="10"/>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="AX2" s="10"/>
-      <c r="AY2" s="10" t="s">
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="7"/>
+      <c r="AX2" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="27"/>
-      <c r="BB2" s="7"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA2" s="7"/>
+      <c r="BB2" s="27"/>
       <c r="BC2" s="7"/>
-      <c r="BD2" s="19" t="s">
+      <c r="BD2" s="7"/>
+      <c r="BE2" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="BE2" s="30" t="s">
-        <v>115</v>
+      <c r="BF2" s="30" t="s">
+        <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>43</v>
       </c>
@@ -1394,77 +1418,80 @@
         <v>64</v>
       </c>
       <c r="W3" s="12"/>
-      <c r="X3" s="12" t="s">
+      <c r="X3" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="Y3" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z3" s="12"/>
       <c r="AA3" s="12"/>
-      <c r="AB3" s="12">
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12">
         <v>1</v>
       </c>
-      <c r="AC3" s="12">
+      <c r="AD3" s="12">
         <v>2</v>
       </c>
-      <c r="AD3" s="12">
+      <c r="AE3" s="12">
         <v>3</v>
       </c>
-      <c r="AE3" s="12">
+      <c r="AF3" s="12">
         <v>4</v>
       </c>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="AH3" s="12" t="s">
-        <v>84</v>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="AI3" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="AJ3" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="AK3" s="23"/>
-      <c r="AL3" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="AM3" s="12"/>
-      <c r="AN3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK3" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL3" s="23"/>
+      <c r="AM3" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="AN3" s="12"/>
+      <c r="AO3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="AO3" s="12" t="s">
+      <c r="AP3" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="AP3" s="12"/>
-      <c r="AQ3" s="14" t="s">
-        <v>91</v>
-      </c>
+      <c r="AQ3" s="12"/>
       <c r="AR3" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="AS3" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT3" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="AT3" s="14"/>
-      <c r="AU3" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="AV3" s="28"/>
-      <c r="AW3" s="15"/>
+      <c r="AU3" s="14"/>
+      <c r="AV3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AW3" s="28"/>
       <c r="AX3" s="15"/>
       <c r="AY3" s="15"/>
-      <c r="AZ3" s="12"/>
-      <c r="BA3" s="28"/>
-      <c r="BB3" s="12"/>
+      <c r="AZ3" s="15"/>
+      <c r="BA3" s="12"/>
+      <c r="BB3" s="28"/>
       <c r="BC3" s="12"/>
-      <c r="BD3" s="20" t="s">
-        <v>99</v>
+      <c r="BD3" s="12"/>
+      <c r="BE3" s="20" t="s">
+        <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:58" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>43</v>
       </c>
@@ -1494,51 +1521,56 @@
       </c>
       <c r="V4" s="12"/>
       <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
+      <c r="X4" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>122</v>
+      </c>
       <c r="Z4" s="12"/>
       <c r="AA4" s="12"/>
       <c r="AB4" s="12"/>
       <c r="AC4" s="12"/>
       <c r="AD4" s="12"/>
       <c r="AE4" s="12"/>
-      <c r="AF4" s="14"/>
+      <c r="AF4" s="12"/>
       <c r="AG4" s="14"/>
-      <c r="AH4" s="12"/>
+      <c r="AH4" s="14"/>
       <c r="AI4" s="12"/>
-      <c r="AJ4" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="AK4" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="AL4" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="AM4" s="12"/>
-      <c r="AN4" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="AO4" s="12"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL4" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM4" s="24" t="s">
+        <v>109</v>
+      </c>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="12" t="s">
+        <v>92</v>
+      </c>
       <c r="AP4" s="12"/>
-      <c r="AQ4" s="14"/>
+      <c r="AQ4" s="12"/>
       <c r="AR4" s="14"/>
       <c r="AS4" s="14"/>
       <c r="AT4" s="14"/>
       <c r="AU4" s="14"/>
-      <c r="AV4" s="28"/>
-      <c r="AW4" s="14"/>
+      <c r="AV4" s="14"/>
+      <c r="AW4" s="28"/>
       <c r="AX4" s="14"/>
       <c r="AY4" s="14"/>
-      <c r="AZ4" s="12"/>
-      <c r="BA4" s="28"/>
-      <c r="BB4" s="12"/>
+      <c r="AZ4" s="14"/>
+      <c r="BA4" s="12"/>
+      <c r="BB4" s="28"/>
       <c r="BC4" s="12"/>
-      <c r="BD4" s="16"/>
+      <c r="BD4" s="12"/>
+      <c r="BE4" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="AJ4" r:id="rId1" xr:uid="{16565EFF-CBEA-AF44-9A5A-AA03399A8B52}"/>
+    <hyperlink ref="AK4" r:id="rId1" xr:uid="{16565EFF-CBEA-AF44-9A5A-AA03399A8B52}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>